<commit_message>
Updated Time Log in Excel Sheet
</commit_message>
<xml_diff>
--- a/auticon SQL Training Assignments and Time Log.xlsx
+++ b/auticon SQL Training Assignments and Time Log.xlsx
@@ -495,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -624,9 +624,6 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2207,7 +2204,9 @@
       </c>
       <c r="D66" s="55"/>
       <c r="E66" s="55"/>
-      <c r="F66" s="56"/>
+      <c r="F66" s="46">
+        <v>360.0</v>
+      </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="48">

</xml_diff>